<commit_message>
test: add test case
</commit_message>
<xml_diff>
--- a/xlsx4conf/test/fixtures/raw.xlsx
+++ b/xlsx4conf/test/fixtures/raw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lance/home/project/something/xmind4conf/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lance/home/project/something/xlsx4conf/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>pf</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>os=ios&amp;pf=uc&amp;entry=school</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>os=ios&amp;pf=uc&amp;entry=market</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -97,7 +93,36 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>系统</t>
+    <t>os</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>os=ios&amp;pf=uc&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=school</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -145,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -168,18 +193,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -460,7 +517,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +527,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -483,96 +540,95 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: cherrio for merged cell
</commit_message>
<xml_diff>
--- a/xlsx4conf/test/fixtures/raw.xlsx
+++ b/xlsx4conf/test/fixtures/raw.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>pf</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,49 +193,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,7 +485,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,10 +511,12 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
@@ -624,11 +594,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: supports dealing with merged cell
</commit_message>
<xml_diff>
--- a/xlsx4conf/test/fixtures/raw.xlsx
+++ b/xlsx4conf/test/fixtures/raw.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>pf</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -193,17 +193,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,7 +517,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:D8"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,12 +543,10 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
@@ -594,10 +624,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: empty cell throw exception
</commit_message>
<xml_diff>
--- a/xlsx4conf/test/fixtures/raw.xlsx
+++ b/xlsx4conf/test/fixtures/raw.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>pf</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -53,10 +53,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>school</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -73,10 +69,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>os=ios&amp;pf=uc&amp;entry=market</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>os=ios&amp;pf=wechat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -94,6 +86,10 @@
   </si>
   <si>
     <t>os</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>os=ios&amp;pf=uc</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -121,7 +117,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>=school</t>
+      <t>=market</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -517,7 +513,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -536,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -544,11 +540,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -560,17 +556,17 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,10 +575,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -590,13 +586,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,10 +613,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>